<commit_message>
Edited Data to Automate
</commit_message>
<xml_diff>
--- a/DataAutomate.xlsx
+++ b/DataAutomate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAAAAAAANAUKA\Node\Job_Application_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8BE9575-3562-468C-A690-C56E406AC2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE6C092-DA07-4109-B79C-6E833B009A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{A20C2D80-053C-42F7-8BCD-392CA0CCCB2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -74,10 +74,16 @@
     <t>Tech Innovations</t>
   </si>
   <si>
-    <t>Minimum 3 lata doświadczenia w Pythonie i tworzeniu aplikacji webowych.</t>
-  </si>
-  <si>
-    <t>Projektowanie, rozwój i utrzymanie aplikacji webowych przy użyciu Python, Django i React.</t>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Minimum 3 years of experience in Python and web application development.</t>
+  </si>
+  <si>
+    <t>Design, develop, and maintain web applications using Python, Django, and React.</t>
   </si>
 </sst>
 </file>
@@ -472,77 +478,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69D20EC-AE61-4932-A90C-4088976820EC}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{ECB55B2A-12D7-4819-B1A7-8BBBF9C15575}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{ECB55B2A-12D7-4819-B1A7-8BBBF9C15575}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>